<commit_message>
Change-Id: Iaceddfc4b699174c119cf8f1861c938ef756719c Signed-off-by: Ibatta <Ibatta@Ibatta-Lap>
</commit_message>
<xml_diff>
--- a/src/com/generic/selenium/testdata/DataSheet.xlsx
+++ b/src/com/generic/selenium/testdata/DataSheet.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="0" windowWidth="17250" windowHeight="5730" activeTab="1"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="17175" windowHeight="6870" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Registration" sheetId="5" r:id="rId2"/>
+    <sheet name="tmp" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="M1:Q14"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>TCID</t>
   </si>
@@ -45,97 +47,100 @@
     <t>postalCode</t>
   </si>
   <si>
+    <t>checkPwd</t>
+  </si>
+  <si>
+    <t>createAccount</t>
+  </si>
+  <si>
+    <t>aa@gg.cc</t>
+  </si>
+  <si>
+    <t>Abeer</t>
+  </si>
+  <si>
+    <t>Alia</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>123456a</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>NumberOfTestCases</t>
+  </si>
+  <si>
+    <t>cc@dd.cc</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>email.errors</t>
+  </si>
+  <si>
+    <t>checkEmail.errors</t>
+  </si>
+  <si>
+    <t>firstName.errors</t>
+  </si>
+  <si>
+    <t>lastName.errors</t>
+  </si>
+  <si>
+    <t>country.errors</t>
+  </si>
+  <si>
+    <t>pwd.errors</t>
+  </si>
+  <si>
+    <t>postalCode.errors</t>
+  </si>
+  <si>
+    <t>checkPwd.errors</t>
+  </si>
+  <si>
+    <t>Please enter a valid email</t>
+  </si>
+  <si>
+    <t>Please confirm your email</t>
+  </si>
+  <si>
+    <t>Please enter a first name</t>
+  </si>
+  <si>
+    <t>Please enter a last name</t>
+  </si>
+  <si>
+    <t>Please enter a Country</t>
+  </si>
+  <si>
+    <t>Please enter a valid zip/postal code.</t>
+  </si>
+  <si>
+    <t>Please enter a strong password (at least 6 characters)</t>
+  </si>
+  <si>
+    <t>Please confirm your password</t>
+  </si>
+  <si>
+    <t>An account already exists for this email address in the Tommy Bahama Main Site. You can use the same account to login to the Tommy Bahama Main Site.</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>checkPwd</t>
-  </si>
-  <si>
-    <t>createAccount</t>
-  </si>
-  <si>
-    <t>aa@gg.cc</t>
-  </si>
-  <si>
-    <t>Abeer</t>
-  </si>
-  <si>
-    <t>Alia</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>123456a</t>
-  </si>
-  <si>
-    <t>Registration</t>
-  </si>
-  <si>
-    <t>NumberOfTestCases</t>
-  </si>
-  <si>
-    <t>cc@dd.cc</t>
-  </si>
-  <si>
-    <t>Sara</t>
-  </si>
-  <si>
-    <t>email.errors</t>
-  </si>
-  <si>
-    <t>checkEmail.errors</t>
-  </si>
-  <si>
-    <t>firstName.errors</t>
-  </si>
-  <si>
-    <t>lastName.errors</t>
-  </si>
-  <si>
-    <t>country.errors</t>
-  </si>
-  <si>
-    <t>pwd.errors</t>
-  </si>
-  <si>
-    <t>postalCode.errors</t>
-  </si>
-  <si>
-    <t>checkPwd.errors</t>
-  </si>
-  <si>
-    <t>Please enter a valid email</t>
-  </si>
-  <si>
-    <t>Please confirm your email</t>
-  </si>
-  <si>
-    <t>Please enter a first name</t>
-  </si>
-  <si>
-    <t>Please enter a last name</t>
-  </si>
-  <si>
-    <t>Please enter a Country</t>
-  </si>
-  <si>
-    <t>Please enter a valid zip/postal code.</t>
-  </si>
-  <si>
-    <t>Please enter a strong password (at least 6 characters)</t>
-  </si>
-  <si>
-    <t>Please confirm your password</t>
-  </si>
-  <si>
-    <t>An account already exists for this email address in the Tommy Bahama Main Site. You can use the same account to login to the Tommy Bahama Main Site.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -378,6 +383,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -413,6 +435,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -610,12 +649,12 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -638,7 +677,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,7 +701,7 @@
     <col min="17" max="17" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -682,67 +721,187 @@
         <v>8</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="F2" s="11">
         <v>44122</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" s="11"/>
       <c r="J2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>37</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" customFormat="1" ht="315" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="11">
+        <v>44122</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -754,19 +913,19 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="14">
         <v>44122</v>
@@ -785,7 +944,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="1"/>
     </row>
@@ -800,28 +959,28 @@
       <c r="H4" s="14"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -831,6 +990,5 @@
     <hyperlink ref="A3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>